<commit_message>
started to add a hsqc CH only experiment, cached java output for quicker response times
</commit_message>
<xml_diff>
--- a/exampleProblems/2-ethyl-1-indanone-bckup/2-ethyl-1-indanone.xlsx
+++ b/exampleProblems/2-ethyl-1-indanone-bckup/2-ethyl-1-indanone.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/2-ethyl-1-indanone-bckup/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_05C51FDA1F2C5DF23FB32D9231BAF82C80E4D26F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A48CC80-0C05-459F-9C18-DF61003716B0}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
     <sheet name="HSQC" sheetId="7" r:id="rId7"/>
     <sheet name="NOESY" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -119,8 +125,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,13 +189,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +241,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -261,6 +275,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -295,9 +310,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -470,19 +486,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -496,14 +512,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -520,15 +541,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.737906072649333</v>
+        <v>7.7379060726493334</v>
       </c>
       <c r="C2">
-        <v>0.9635095233053554</v>
+        <v>0.96350952330535544</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -540,15 +561,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>7.567027089863733</v>
+        <v>7.5670270898637328</v>
       </c>
       <c r="C3">
-        <v>0.9988670990901746</v>
+        <v>0.99886709909017457</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -560,15 +581,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7.449204824899009</v>
+        <v>7.4492048248990086</v>
       </c>
       <c r="C4">
-        <v>0.9962538806992282</v>
+        <v>0.99625388069922816</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -580,15 +601,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7.349303067688013</v>
+        <v>7.3493030676880133</v>
       </c>
       <c r="C5">
-        <v>1.011963343602272</v>
+        <v>1.0119633436022719</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -600,15 +621,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3.308352426774753</v>
+        <v>3.3083524267747531</v>
       </c>
       <c r="C6">
-        <v>0.9995099736473627</v>
+        <v>0.99950997364736271</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -620,15 +641,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2.812059483796793</v>
+        <v>2.8120594837967929</v>
       </c>
       <c r="C7">
-        <v>0.9983553113955096</v>
+        <v>0.99835531139550959</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -640,12 +661,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2.606421855689738</v>
+        <v>2.6064218556897378</v>
       </c>
       <c r="C8">
         <v>1.003196264608754</v>
@@ -660,15 +681,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.965223914004773</v>
+        <v>1.9652239140047729</v>
       </c>
       <c r="C9">
-        <v>1.006332741900848</v>
+        <v>1.0063327419008481</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -680,15 +701,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1.533649712037166</v>
+        <v>1.5336497120371659</v>
       </c>
       <c r="C10">
-        <v>1.025149996411519</v>
+        <v>1.0251499964115189</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -700,12 +721,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1.001752588817867</v>
+        <v>1.0017525888178671</v>
       </c>
       <c r="C11">
         <v>2.996861865338976</v>
@@ -726,14 +747,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -750,7 +771,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -758,7 +779,7 @@
         <v>7.738519669434182</v>
       </c>
       <c r="C2">
-        <v>0.9700662258106406</v>
+        <v>0.97006622581064061</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -770,15 +791,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>7.567639640676065</v>
+        <v>7.5676396406760649</v>
       </c>
       <c r="C3">
-        <v>1.464692329237974</v>
+        <v>1.4646923292379741</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -790,12 +811,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7.449801876471231</v>
+        <v>7.4498018764712306</v>
       </c>
       <c r="C4">
         <v>1.334290088698737</v>
@@ -810,15 +831,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3.308678727534115</v>
+        <v>3.3086787275341152</v>
       </c>
       <c r="C5">
-        <v>4.698744596232448</v>
+        <v>4.6987445962324479</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -830,15 +851,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2.812309654526748</v>
+        <v>2.8123096545267479</v>
       </c>
       <c r="C6">
-        <v>5.479107090614503</v>
+        <v>5.4791070906145034</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -850,7 +871,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -858,7 +879,7 @@
         <v>2.606577722472295</v>
       </c>
       <c r="C7">
-        <v>2.076579484476073</v>
+        <v>2.0765794844760732</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -870,15 +891,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1.965452325708671</v>
+        <v>1.9654523257086709</v>
       </c>
       <c r="C8">
-        <v>3.800910832420514</v>
+        <v>3.8009108324205139</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -890,15 +911,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.953786156836632</v>
+        <v>1.9537861568366319</v>
       </c>
       <c r="C9">
-        <v>0.9620083589913344</v>
+        <v>0.96200835899133441</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -910,7 +931,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -918,7 +939,7 @@
         <v>1.542310438563758</v>
       </c>
       <c r="C10">
-        <v>1.516589538238677</v>
+        <v>1.5165895382386769</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -930,15 +951,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1.001858396199719</v>
+        <v>1.0018583961997189</v>
       </c>
       <c r="C11">
-        <v>11.03381826525854</v>
+        <v>11.033818265258541</v>
       </c>
       <c r="D11">
         <v>11</v>
@@ -950,15 +971,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.9939790313613932</v>
+        <v>0.99397903136139321</v>
       </c>
       <c r="C12">
-        <v>1.663193190020552</v>
+        <v>1.6631931900205521</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -976,14 +997,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -994,7 +1015,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1002,46 +1023,46 @@
         <v>208.9336573688492</v>
       </c>
       <c r="C2">
-        <v>381.3484273992452</v>
+        <v>381.34842739924522</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>153.8100376399912</v>
+        <v>153.81003763999121</v>
       </c>
       <c r="C3">
-        <v>737.2143370064695</v>
+        <v>737.21433700646946</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>136.9548804575541</v>
+        <v>136.95488045755411</v>
       </c>
       <c r="C4">
-        <v>542.3864653859198</v>
+        <v>542.38646538591979</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>134.5884480174205</v>
+        <v>134.58844801742049</v>
       </c>
       <c r="C5">
         <v>2086.501280496142</v>
@@ -1050,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1058,13 +1079,13 @@
         <v>127.2743508502364</v>
       </c>
       <c r="C6">
-        <v>2093.507743797035</v>
+        <v>2093.5077437970349</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1078,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1092,54 +1113,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>48.74270426301496</v>
+        <v>48.742704263014957</v>
       </c>
       <c r="C9">
-        <v>2002.161458938643</v>
+        <v>2002.1614589386429</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>32.31753922066989</v>
+        <v>32.317539220669893</v>
       </c>
       <c r="C10">
-        <v>2194.061391729568</v>
+        <v>2194.0613917295682</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>24.45272702583003</v>
+        <v>24.452727025830029</v>
       </c>
       <c r="C11">
-        <v>2280.357409187266</v>
+        <v>2280.3574091872661</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>11.58170032407751</v>
+        <v>11.581700324077509</v>
       </c>
       <c r="C12">
         <v>2246.653503582123</v>
@@ -1154,14 +1175,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1175,32 +1196,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.738797423150298</v>
+        <v>7.7387974231502978</v>
       </c>
       <c r="C2">
-        <v>7.35183187328886</v>
+        <v>7.3518318732888597</v>
       </c>
       <c r="D2">
-        <v>0.8134216666221619</v>
+        <v>0.81342166662216187</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>7.56953110048025</v>
+        <v>7.5695311004802504</v>
       </c>
       <c r="C3">
-        <v>7.451800333332647</v>
+        <v>7.4518003333326472</v>
       </c>
       <c r="D3">
         <v>1.738711953163147</v>
@@ -1209,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1217,16 +1238,16 @@
         <v>7.568104698884718</v>
       </c>
       <c r="C4">
-        <v>7.35183187328886</v>
+        <v>7.3518318732888597</v>
       </c>
       <c r="D4">
-        <v>0.2911712229251862</v>
+        <v>0.29117122292518621</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1234,16 +1255,16 @@
         <v>7.448286964859852</v>
       </c>
       <c r="C5">
-        <v>7.449420131903032</v>
+        <v>7.4494201319030324</v>
       </c>
       <c r="D5">
-        <v>0.3366815745830536</v>
+        <v>0.33668157458305359</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1251,7 +1272,7 @@
         <v>3.308523412472284</v>
       </c>
       <c r="C6">
-        <v>2.82808211611824</v>
+        <v>2.8280821161182401</v>
       </c>
       <c r="D6">
         <v>1.602514386177063</v>
@@ -1260,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1271,55 +1292,55 @@
         <v>2.608192159735208</v>
       </c>
       <c r="D7">
-        <v>0.09335356205701828</v>
+        <v>9.335356205701828E-2</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2.811098274247846</v>
+        <v>2.8110982742478461</v>
       </c>
       <c r="C8">
         <v>2.811470139162441</v>
       </c>
       <c r="D8">
-        <v>0.3049026429653168</v>
+        <v>0.30490264296531677</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2.810631753507861</v>
+        <v>2.8106317535078609</v>
       </c>
       <c r="C9">
-        <v>2.609643643128534</v>
+        <v>2.6096436431285341</v>
       </c>
       <c r="D9">
-        <v>0.01834593899548054</v>
+        <v>1.8345938995480541E-2</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2.6086036350616</v>
+        <v>2.6086036350616002</v>
       </c>
       <c r="C10">
-        <v>2.609643643128534</v>
+        <v>2.6096436431285341</v>
       </c>
       <c r="D10">
         <v>0.341642826795578</v>
@@ -1328,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1339,41 +1360,41 @@
         <v>1.531134967369663</v>
       </c>
       <c r="D11">
-        <v>0.04948503896594048</v>
+        <v>4.9485038965940482E-2</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1.968065220244318</v>
+        <v>1.9680652202443181</v>
       </c>
       <c r="C12">
-        <v>1.002534855406425</v>
+        <v>1.0025348554064251</v>
       </c>
       <c r="D12">
-        <v>0.2910004556179047</v>
+        <v>0.29100045561790472</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1.532394293753809</v>
+        <v>1.5323942937538091</v>
       </c>
       <c r="C13">
-        <v>1.008170223277162</v>
+        <v>1.0081702232771621</v>
       </c>
       <c r="D13">
-        <v>0.77091383934021</v>
+        <v>0.77091383934020996</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1385,14 +1406,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1406,262 +1427,262 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.739081072734923</v>
+        <v>7.7390810727349226</v>
       </c>
       <c r="C2">
-        <v>134.5537793157619</v>
+        <v>134.55377931576189</v>
       </c>
       <c r="D2">
-        <v>0.03238219022750854</v>
+        <v>3.2382190227508538E-2</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>7.739059485744913</v>
+        <v>7.7390594857449129</v>
       </c>
       <c r="C3">
-        <v>153.7370790049119</v>
+        <v>153.73707900491189</v>
       </c>
       <c r="D3">
-        <v>0.0161228384822607</v>
+        <v>1.6122838482260701E-2</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7.737701346272939</v>
+        <v>7.7377013462729387</v>
       </c>
       <c r="C4">
-        <v>208.9639245366668</v>
+        <v>208.96392453666681</v>
       </c>
       <c r="D4">
-        <v>0.01698123849928379</v>
+        <v>1.6981238499283791E-2</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7.56654632869329</v>
+        <v>7.5665463286932901</v>
       </c>
       <c r="C5">
         <v>123.7884527970556</v>
       </c>
       <c r="D5">
-        <v>0.0313577800989151</v>
+        <v>3.13577800989151E-2</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7.56654632869329</v>
+        <v>7.5665463286932901</v>
       </c>
       <c r="C6">
-        <v>153.9206818618219</v>
+        <v>153.92068186182189</v>
       </c>
       <c r="D6">
-        <v>0.02967634797096252</v>
+        <v>2.9676347970962521E-2</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>7.450009008259263</v>
+        <v>7.4500090082592632</v>
       </c>
       <c r="C7">
-        <v>32.34306999766169</v>
+        <v>32.343069997661694</v>
       </c>
       <c r="D7">
-        <v>0.0139024443924427</v>
+        <v>1.39024443924427E-2</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7.44956698976257</v>
+        <v>7.4495669897625696</v>
       </c>
       <c r="C8">
-        <v>137.0113724664344</v>
+        <v>137.01137246643441</v>
       </c>
       <c r="D8">
-        <v>0.0150699932128191</v>
+        <v>1.5069993212819099E-2</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>7.448954187158241</v>
+        <v>7.4489541871582414</v>
       </c>
       <c r="C9">
         <v>127.2596674358505</v>
       </c>
       <c r="D9">
-        <v>0.01846521161496639</v>
+        <v>1.8465211614966389E-2</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>7.448393284020789</v>
+        <v>7.4483932840207894</v>
       </c>
       <c r="C10">
-        <v>134.6606311918781</v>
+        <v>134.66063119187811</v>
       </c>
       <c r="D10">
-        <v>0.05258383601903915</v>
+        <v>5.2583836019039147E-2</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>7.347454590227726</v>
+        <v>7.3474545902277262</v>
       </c>
       <c r="C11">
-        <v>137.0915113735215</v>
+        <v>137.09151137352151</v>
       </c>
       <c r="D11">
-        <v>0.02995355054736137</v>
+        <v>2.995355054736137E-2</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>3.310479993153229</v>
+        <v>3.3104799931532289</v>
       </c>
       <c r="C12">
-        <v>48.77770804469969</v>
+        <v>48.777708044699693</v>
       </c>
       <c r="D12">
-        <v>0.0426684282720089</v>
+        <v>4.2668428272008903E-2</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3.309900830653378</v>
+        <v>3.3099008306533779</v>
       </c>
       <c r="C13">
-        <v>136.9268355678205</v>
+        <v>136.92683556782049</v>
       </c>
       <c r="D13">
-        <v>0.023663479834795</v>
+        <v>2.3663479834795002E-2</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>3.309900830653378</v>
+        <v>3.3099008306533779</v>
       </c>
       <c r="C14">
         <v>126.5593822832416</v>
       </c>
       <c r="D14">
-        <v>0.01754710450768471</v>
+        <v>1.7547104507684711E-2</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>3.309760172323564</v>
+        <v>3.3097601723235641</v>
       </c>
       <c r="C15">
-        <v>153.8654813617698</v>
+        <v>153.86548136176981</v>
       </c>
       <c r="D15">
-        <v>0.06188980117440224</v>
+        <v>6.1889801174402237E-2</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>3.308706688916356</v>
+        <v>3.3087066889163559</v>
       </c>
       <c r="C16">
-        <v>24.4519070661565</v>
+        <v>24.451907066156501</v>
       </c>
       <c r="D16">
-        <v>0.01909291930496693</v>
+        <v>1.909291930496693E-2</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1672,132 +1693,132 @@
         <v>208.9329448985504</v>
       </c>
       <c r="D17">
-        <v>0.07332679629325867</v>
+        <v>7.3326796293258667E-2</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2.813698044492167</v>
+        <v>2.8136980444921669</v>
       </c>
       <c r="C18">
-        <v>153.8570462955456</v>
+        <v>153.85704629554559</v>
       </c>
       <c r="D18">
-        <v>0.0137866223230958</v>
+        <v>1.37866223230958E-2</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>2.813109179294286</v>
+        <v>2.8131091792942859</v>
       </c>
       <c r="C19">
-        <v>24.4979059530839</v>
+        <v>24.497905953083901</v>
       </c>
       <c r="D19">
-        <v>0.02038756757974625</v>
+        <v>2.038756757974625E-2</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>2.813109179294286</v>
+        <v>2.8131091792942859</v>
       </c>
       <c r="C20">
-        <v>48.78647067176841</v>
+        <v>48.786470671768413</v>
       </c>
       <c r="D20">
-        <v>0.01470457203686237</v>
+        <v>1.470457203686237E-2</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>2.812836883622136</v>
+        <v>2.8128368836221358</v>
       </c>
       <c r="C21">
         <v>126.5856682826024</v>
       </c>
       <c r="D21">
-        <v>0.003435649443417788</v>
+        <v>3.435649443417788E-3</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>2.812467814677838</v>
+        <v>2.8124678146778379</v>
       </c>
       <c r="C22">
-        <v>137.023221274763</v>
+        <v>137.02322127476299</v>
       </c>
       <c r="D22">
-        <v>0.007866300642490387</v>
+        <v>7.866300642490387E-3</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>2.812467814677838</v>
+        <v>2.8124678146778379</v>
       </c>
       <c r="C23">
-        <v>134.5519343546135</v>
+        <v>134.55193435461351</v>
       </c>
       <c r="D23">
-        <v>0.002547277836129069</v>
+        <v>2.5472778361290689E-3</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>2.606833314250037</v>
+        <v>2.6068333142500371</v>
       </c>
       <c r="C24">
-        <v>24.4177333924053</v>
+        <v>24.417733392405299</v>
       </c>
       <c r="D24">
-        <v>0.04327566176652908</v>
+        <v>4.3275661766529083E-2</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1808,81 +1829,81 @@
         <v>11.6481548911204</v>
       </c>
       <c r="D25">
-        <v>0.01824538037180901</v>
+        <v>1.8245380371809009E-2</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>2.606521544280026</v>
+        <v>2.6065215442800258</v>
       </c>
       <c r="C26">
         <v>209.0903490562938</v>
       </c>
       <c r="D26">
-        <v>0.03120999038219452</v>
+        <v>3.1209990382194519E-2</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>2.606511376109262</v>
+        <v>2.6065113761092622</v>
       </c>
       <c r="C27">
         <v>32.32271055986736</v>
       </c>
       <c r="D27">
-        <v>0.0395892933011055</v>
+        <v>3.9589293301105499E-2</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>2.606162450172059</v>
+        <v>2.6061624501720591</v>
       </c>
       <c r="C28">
-        <v>153.7633380356303</v>
+        <v>153.76333803563031</v>
       </c>
       <c r="D28">
-        <v>0.02524148114025593</v>
+        <v>2.5241481140255932E-2</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>1.9668695430369</v>
+        <v>1.9668695430369001</v>
       </c>
       <c r="C29">
-        <v>32.12927507067344</v>
+        <v>32.129275070673437</v>
       </c>
       <c r="D29">
-        <v>0.0381791926920414</v>
+        <v>3.8179192692041397E-2</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1890,16 +1911,16 @@
         <v>1.966460574747271</v>
       </c>
       <c r="C30">
-        <v>48.79358066930958</v>
+        <v>48.793580669309577</v>
       </c>
       <c r="D30">
-        <v>0.01629587635397911</v>
+        <v>1.6295876353979111E-2</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1907,16 +1928,16 @@
         <v>1.966457890995758</v>
       </c>
       <c r="C31">
-        <v>209.0466470408419</v>
+        <v>209.04664704084189</v>
       </c>
       <c r="D31">
-        <v>0.01562971621751785</v>
+        <v>1.5629716217517849E-2</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1924,50 +1945,50 @@
         <v>1.964279410535918</v>
       </c>
       <c r="C32">
-        <v>11.6299719915564</v>
+        <v>11.629971991556401</v>
       </c>
       <c r="D32">
-        <v>0.007152247242629528</v>
+        <v>7.152247242629528E-3</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>1.53236041616988</v>
+        <v>1.5323604161698801</v>
       </c>
       <c r="C33">
-        <v>208.9368506794067</v>
+        <v>208.93685067940669</v>
       </c>
       <c r="D33">
-        <v>0.02744573354721069</v>
+        <v>2.744573354721069E-2</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1.532059048812357</v>
+        <v>1.5320590488123571</v>
       </c>
       <c r="C34">
-        <v>11.56343943273549</v>
+        <v>11.563439432735491</v>
       </c>
       <c r="D34">
-        <v>0.01703412458300591</v>
+        <v>1.7034124583005909E-2</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1978,13 +1999,13 @@
         <v>48.77003817892794</v>
       </c>
       <c r="D35">
-        <v>0.2883979976177216</v>
+        <v>0.28839799761772161</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2007,14 +2028,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
@@ -2028,15 +2049,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.73749078103152</v>
+        <v>7.7374907810315197</v>
       </c>
       <c r="C2">
-        <v>123.8178255995061</v>
+        <v>123.81782559950609</v>
       </c>
       <c r="D2">
         <v>0.491100013256073</v>
@@ -2045,92 +2066,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>7.566955617395458</v>
+        <v>7.5669556173954584</v>
       </c>
       <c r="C3">
-        <v>134.5886670549037</v>
+        <v>134.58866705490371</v>
       </c>
       <c r="D3">
-        <v>0.4672920107841492</v>
+        <v>0.46729201078414923</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7.449675279677171</v>
+        <v>7.4496752796771712</v>
       </c>
       <c r="C4">
         <v>126.5261790589672</v>
       </c>
       <c r="D4">
-        <v>0.5302392244338989</v>
+        <v>0.53023922443389893</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7.34852249666585</v>
+        <v>7.3485224966658498</v>
       </c>
       <c r="C5">
-        <v>127.2730737912241</v>
+        <v>127.27307379122411</v>
       </c>
       <c r="D5">
-        <v>0.7416589260101318</v>
+        <v>0.74165892601013184</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3.310743089047947</v>
+        <v>3.3107430890479468</v>
       </c>
       <c r="C6">
-        <v>32.3181199391579</v>
+        <v>32.318119939157903</v>
       </c>
       <c r="D6">
-        <v>-0.3162756562232971</v>
+        <v>-0.31627565622329712</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2.812489829649986</v>
+        <v>2.8124898296499858</v>
       </c>
       <c r="C7">
-        <v>32.3181199391579</v>
+        <v>32.318119939157903</v>
       </c>
       <c r="D7">
-        <v>-0.007556002587080002</v>
+        <v>-7.5560025870800018E-3</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2141,47 +2162,47 @@
         <v>48.74709494448755</v>
       </c>
       <c r="D8">
-        <v>0.5715267658233643</v>
+        <v>0.57152676582336426</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.965674184396632</v>
+        <v>1.9656741843966321</v>
       </c>
       <c r="C9">
         <v>24.45345507399847</v>
       </c>
       <c r="D9">
-        <v>-0.3529969453811646</v>
+        <v>-0.35299694538116461</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1.532886961804531</v>
+        <v>1.5328869618045311</v>
       </c>
       <c r="C10">
         <v>24.45345507399847</v>
       </c>
       <c r="D10">
-        <v>-0.3348827660083771</v>
+        <v>-0.33488276600837708</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2192,7 +2213,7 @@
         <v>11.58358396648709</v>
       </c>
       <c r="D11">
-        <v>2.177265167236328</v>
+        <v>2.1772651672363281</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2204,14 +2225,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>